<commit_message>
cleaned and processed data from 201819 to 201516 and started neural net code
</commit_message>
<xml_diff>
--- a/data/formatted/basicdata201617.xlsx
+++ b/data/formatted/basicdata201617.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\petri\Documents\CS-4641\machine-learning-madness\data\formatted\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meha\Documents\machine-learning-madness\data\formatted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6B067A-BC7E-4490-B142-1262B1606489}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BA84F7F4-7F78-43C2-93C5-7D02D159B496}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19422" windowHeight="10422"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -255,9 +254,6 @@
     <t>Rhode Island</t>
   </si>
   <si>
-    <t>Saint Mary's (CA)</t>
-  </si>
-  <si>
     <t>Seton Hall</t>
   </si>
   <si>
@@ -316,12 +312,15 @@
   </si>
   <si>
     <t>Xavier</t>
+  </si>
+  <si>
+    <t>Saint Mary's</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -666,16 +665,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{340468EC-8914-4D06-B0A4-FB4231657B03}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AA69"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B49" sqref="A1:AA69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -758,7 +757,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>13</v>
       </c>
@@ -841,7 +840,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>17</v>
       </c>
@@ -924,7 +923,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>22</v>
       </c>
@@ -1007,7 +1006,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>34</v>
       </c>
@@ -1090,7 +1089,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>36</v>
       </c>
@@ -1173,7 +1172,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>41</v>
       </c>
@@ -1256,7 +1255,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>56</v>
       </c>
@@ -1339,7 +1338,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>69</v>
       </c>
@@ -1422,7 +1421,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>72</v>
       </c>
@@ -1505,7 +1504,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>80</v>
       </c>
@@ -1588,7 +1587,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>83</v>
       </c>
@@ -1671,7 +1670,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>94</v>
       </c>
@@ -1754,7 +1753,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>96</v>
       </c>
@@ -1837,7 +1836,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>97</v>
       </c>
@@ -1920,7 +1919,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>109</v>
       </c>
@@ -2003,7 +2002,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>131</v>
       </c>
@@ -2086,7 +2085,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>132</v>
       </c>
@@ -2169,7 +2168,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>137</v>
       </c>
@@ -2252,7 +2251,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>140</v>
       </c>
@@ -2335,7 +2334,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>141</v>
       </c>
@@ -2418,7 +2417,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>143</v>
       </c>
@@ -2501,7 +2500,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>144</v>
       </c>
@@ -2584,7 +2583,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>158</v>
       </c>
@@ -2667,7 +2666,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>165</v>
       </c>
@@ -2750,7 +2749,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>169</v>
       </c>
@@ -2833,7 +2832,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>175</v>
       </c>
@@ -2916,7 +2915,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>177</v>
       </c>
@@ -2999,7 +2998,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>178</v>
       </c>
@@ -3082,7 +3081,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>179</v>
       </c>
@@ -3165,7 +3164,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>181</v>
       </c>
@@ -3248,7 +3247,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>193</v>
       </c>
@@ -3331,7 +3330,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>199</v>
       </c>
@@ -3414,7 +3413,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>201</v>
       </c>
@@ -3497,7 +3496,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>203</v>
       </c>
@@ -3580,7 +3579,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>210</v>
       </c>
@@ -3663,7 +3662,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>213</v>
       </c>
@@ -3746,7 +3745,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <v>214</v>
       </c>
@@ -3829,7 +3828,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>216</v>
       </c>
@@ -3912,7 +3911,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>224</v>
       </c>
@@ -3995,7 +3994,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>226</v>
       </c>
@@ -4078,7 +4077,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>227</v>
       </c>
@@ -4161,7 +4160,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>231</v>
       </c>
@@ -4244,7 +4243,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>236</v>
       </c>
@@ -4327,7 +4326,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <v>246</v>
       </c>
@@ -4410,7 +4409,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <v>247</v>
       </c>
@@ -4493,7 +4492,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
         <v>248</v>
       </c>
@@ -4576,7 +4575,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <v>251</v>
       </c>
@@ -4659,12 +4658,12 @@
         <v>725</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <v>262</v>
       </c>
       <c r="B49" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="C49">
         <v>29</v>
@@ -4742,12 +4741,12 @@
         <v>512</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <v>273</v>
       </c>
       <c r="B50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C50">
         <v>21</v>
@@ -4825,12 +4824,12 @@
         <v>613</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <v>278</v>
       </c>
       <c r="B51" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C51">
         <v>26</v>
@@ -4908,12 +4907,12 @@
         <v>751</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
         <v>279</v>
       </c>
       <c r="B52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C52">
         <v>18</v>
@@ -4991,12 +4990,12 @@
         <v>584</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
         <v>284</v>
       </c>
       <c r="B53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C53">
         <v>26</v>
@@ -5074,12 +5073,12 @@
         <v>571</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
         <v>287</v>
       </c>
       <c r="B54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C54">
         <v>30</v>
@@ -5157,12 +5156,12 @@
         <v>506</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
         <v>311</v>
       </c>
       <c r="B55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C55">
         <v>23</v>
@@ -5240,12 +5239,12 @@
         <v>607</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
         <v>317</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C56">
         <v>22</v>
@@ -5323,12 +5322,12 @@
         <v>654</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
         <v>320</v>
       </c>
       <c r="B57" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C57">
         <v>31</v>
@@ -5406,12 +5405,12 @@
         <v>583</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
         <v>325</v>
       </c>
       <c r="B58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C58">
         <v>19</v>
@@ -5489,12 +5488,12 @@
         <v>581</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
         <v>326</v>
       </c>
       <c r="B59" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C59">
         <v>29</v>
@@ -5572,12 +5571,12 @@
         <v>555</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
         <v>327</v>
       </c>
       <c r="B60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C60">
         <v>32</v>
@@ -5655,12 +5654,12 @@
         <v>515</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A61">
         <v>328</v>
       </c>
       <c r="B61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C61">
         <v>26</v>
@@ -5738,12 +5737,12 @@
         <v>728</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
         <v>330</v>
       </c>
       <c r="B62" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C62">
         <v>22</v>
@@ -5821,12 +5820,12 @@
         <v>543</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
         <v>331</v>
       </c>
       <c r="B63" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C63">
         <v>23</v>
@@ -5904,12 +5903,12 @@
         <v>556</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
         <v>333</v>
       </c>
       <c r="B64" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C64">
         <v>19</v>
@@ -5987,12 +5986,12 @@
         <v>668</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
         <v>337</v>
       </c>
       <c r="B65" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C65">
         <v>28</v>
@@ -6070,12 +6069,12 @@
         <v>756</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
         <v>342</v>
       </c>
       <c r="B66" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C66">
         <v>31</v>
@@ -6153,12 +6152,12 @@
         <v>676</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A67">
         <v>344</v>
       </c>
       <c r="B67" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C67">
         <v>26</v>
@@ -6236,12 +6235,12 @@
         <v>605</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
         <v>345</v>
       </c>
       <c r="B68" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C68">
         <v>27</v>
@@ -6319,12 +6318,12 @@
         <v>602</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
         <v>349</v>
       </c>
       <c r="B69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C69">
         <v>24</v>

</xml_diff>